<commit_message>
further edits to SinghRamesh_2023
the submitted data had some odd units, which I've fixed manually
</commit_message>
<xml_diff>
--- a/data/SinghRamesh_2023/raw/SinghRamesh_etal2023_Biomass_RGR_metadatafile.xlsx
+++ b/data/SinghRamesh_2023/raw/SinghRamesh_etal2023_Biomass_RGR_metadatafile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uqasin21/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arunr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BEA920-0D16-3A49-8252-02964370140B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B269D823-A913-4135-8595-890241A11441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6340" yWindow="8300" windowWidth="27240" windowHeight="16440" xr2:uid="{6889CEA8-909B-0D4F-A559-EF2B87E58AAC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6889CEA8-909B-0D4F-A559-EF2B87E58AAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="133">
   <si>
     <t>POT</t>
   </si>
@@ -155,12 +155,6 @@
     <t>%N</t>
   </si>
   <si>
-    <t>Leaf_C_area</t>
-  </si>
-  <si>
-    <t>Leaf_N_Area</t>
-  </si>
-  <si>
     <t>Soil_N(%)</t>
   </si>
   <si>
@@ -351,12 +345,6 @@
   </si>
   <si>
     <t>Total nitrogen (%)</t>
-  </si>
-  <si>
-    <t>Leaf carbon content per unit leaf area</t>
-  </si>
-  <si>
-    <t>Leaf nitrogen content per unit leaf area</t>
   </si>
   <si>
     <t>Total soil N (%)</t>
@@ -436,6 +424,24 @@
   </si>
   <si>
     <t>Publication</t>
+  </si>
+  <si>
+    <t>Leaf nitrogen content per unit leaf area (calculated as : ((mass of Nitrogen/SLA)*1000) in kg m^2)</t>
+  </si>
+  <si>
+    <t>Leaf phosphorous content per unit leaf area (calculated as : ((mass of Phosphorous/SLA)*1000) in kg m^2)</t>
+  </si>
+  <si>
+    <t>Leaf_P_Area_kg_m-2</t>
+  </si>
+  <si>
+    <t>Leaf_N_Area_kg_m-2</t>
+  </si>
+  <si>
+    <t>%P</t>
+  </si>
+  <si>
+    <t>Total leaf phosphorous (%)</t>
   </si>
 </sst>
 </file>
@@ -479,11 +485,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -799,550 +808,559 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A93A058-61ED-7541-93FF-3B30D57DA466}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="182.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="372" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="3">
         <v>3.1427999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>38</v>
       </c>
       <c r="B40" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>129</v>
+      </c>
+      <c r="B41" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>130</v>
+      </c>
+      <c r="B42" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>44</v>
-      </c>
-      <c r="B46" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>45</v>
-      </c>
-      <c r="B47" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>46</v>
-      </c>
-      <c r="B48" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>47</v>
-      </c>
-      <c r="B49" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>48</v>
-      </c>
-      <c r="B50" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B51" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>131</v>
+      </c>
+      <c r="B55" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>51</v>
+      </c>
+      <c r="B56" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>50</v>
-      </c>
-      <c r="B52" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>52</v>
+      </c>
+      <c r="B57" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>51</v>
-      </c>
-      <c r="B53" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>53</v>
+      </c>
+      <c r="B58" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>52</v>
-      </c>
-      <c r="B54" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>54</v>
+      </c>
+      <c r="B59" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>55</v>
+      </c>
+      <c r="B60" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>56</v>
+      </c>
+      <c r="B61" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>53</v>
-      </c>
-      <c r="B55" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>57</v>
+      </c>
+      <c r="B62" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B56" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>58</v>
+      </c>
+      <c r="B63" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>55</v>
-      </c>
-      <c r="B57" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>59</v>
+      </c>
+      <c r="B64" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>56</v>
-      </c>
-      <c r="B58" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>57</v>
-      </c>
-      <c r="B59" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>58</v>
-      </c>
-      <c r="B60" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>60</v>
+      </c>
+      <c r="B65" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>59</v>
-      </c>
-      <c r="B61" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>61</v>
+      </c>
+      <c r="B66" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>60</v>
-      </c>
-      <c r="B62" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>62</v>
+      </c>
+      <c r="B67" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>61</v>
-      </c>
-      <c r="B63" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>62</v>
-      </c>
-      <c r="B64" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>63</v>
-      </c>
-      <c r="B65" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>64</v>
-      </c>
-      <c r="B66" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>